<commit_message>
added setcleared to unknwon button
</commit_message>
<xml_diff>
--- a/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
+++ b/sormas-api/src/main/resources/doc/SORMAS_User_Rights.xlsx
@@ -63,7 +63,7 @@
     <t>National Observer</t>
   </si>
   <si>
-    <t>State Observer</t>
+    <t>Region Observer</t>
   </si>
   <si>
     <t>District Observer</t>
@@ -108,7 +108,7 @@
     <t>District</t>
   </si>
   <si>
-    <t>Health facility</t>
+    <t>Facility</t>
   </si>
   <si>
     <t>Community</t>
@@ -501,7 +501,7 @@
     <t>SORMAS Version</t>
   </si>
   <si>
-    <t>1.46.0-SNAPSHOT</t>
+    <t>1.47.0-SNAPSHOT</t>
   </si>
 </sst>
 </file>

</xml_diff>